<commit_message>
chore(landing): save state before change landing
</commit_message>
<xml_diff>
--- a/docs/marketing/emaile-firmy.xlsx
+++ b/docs/marketing/emaile-firmy.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anteqkois/Code/Projects/me/linkerry/docs/marketing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1D30630-CADB-0849-9E4F-ECBA8B143848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F144FB-DAE7-A04C-B4F6-1846BF31268C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" xr2:uid="{0D299B25-0D75-CB42-9587-9925ADB6A02D}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,9 +36,530 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="172">
+  <si>
+    <t>Nazwa</t>
+  </si>
+  <si>
+    <t>strona</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>odpowiedź</t>
+  </si>
+  <si>
+    <t>współpraca</t>
+  </si>
+  <si>
+    <t>biuro@reflect.pl</t>
+  </si>
+  <si>
+    <t>https://www.reflect.pl/kontakt.html</t>
+  </si>
+  <si>
+    <t>Reflect</t>
+  </si>
+  <si>
+    <t>biuro@4lans.pl</t>
+  </si>
+  <si>
+    <t>https://4lans.pl/kontakt</t>
+  </si>
+  <si>
+    <t>4lans</t>
+  </si>
+  <si>
+    <t>branża</t>
+  </si>
+  <si>
+    <t>Produkcja odzieży</t>
+  </si>
+  <si>
+    <t>Lillow</t>
+  </si>
+  <si>
+    <t>biuro@lillow.pl</t>
+  </si>
+  <si>
+    <t>https://lillow.pl/strony/kontakt</t>
+  </si>
+  <si>
+    <t>Rascal</t>
+  </si>
+  <si>
+    <t>hello@rascalindustry.eu</t>
+  </si>
+  <si>
+    <t>https://www.rascalindustry.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>MerchUp</t>
+  </si>
+  <si>
+    <t>hello@merchup.com</t>
+  </si>
+  <si>
+    <t>https://www.merchup.com/skontaktuj-sie/</t>
+  </si>
+  <si>
+    <t>https://www.zafirmowani.pl/baza-firm/produkcja-odziezy</t>
+  </si>
+  <si>
+    <t>Artdress</t>
+  </si>
+  <si>
+    <t>info@artdress.com.pl</t>
+  </si>
+  <si>
+    <t>https://www.artdress.com.pl/kontakt</t>
+  </si>
+  <si>
+    <t>https://panoramafirm.pl/producent_odzie%C5%BCy</t>
+  </si>
+  <si>
+    <t>Elastic</t>
+  </si>
+  <si>
+    <t>elastic@elastic.com.pl</t>
+  </si>
+  <si>
+    <t>https://elastic.com.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>E-hurtowo.eu</t>
+  </si>
+  <si>
+    <t>https://www.e-hurtowo.eu/kontakt-f-1.html</t>
+  </si>
+  <si>
+    <t>biuro@e-hurtowo.eu</t>
+  </si>
+  <si>
+    <t>Joan</t>
+  </si>
+  <si>
+    <t>https://joan.com.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>https://ratingcaptain.com/pl/blog/made-in-poland-ranking-najlepszych-polskich-marek-odziezowych</t>
+  </si>
+  <si>
+    <t>Fabris</t>
+  </si>
+  <si>
+    <t>fabris@fabris.pl</t>
+  </si>
+  <si>
+    <t>https://fabris.pl/</t>
+  </si>
+  <si>
+    <t>Fabryka bluz</t>
+  </si>
+  <si>
+    <t>info@fabrykabluz.pl</t>
+  </si>
+  <si>
+    <t>https://www.fabrykabluz.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>https://www.bluzup.com/kontakt/</t>
+  </si>
+  <si>
+    <t>BluzUp</t>
+  </si>
+  <si>
+    <t>hello@bluzup.com</t>
+  </si>
+  <si>
+    <t>Fabor</t>
+  </si>
+  <si>
+    <t>biuro@fabor.pl</t>
+  </si>
+  <si>
+    <t>joan@joan.com.pl</t>
+  </si>
+  <si>
+    <t>https://www.fabor.pl/en/contact/</t>
+  </si>
+  <si>
+    <t>https://blekitna.com/webpage/kontakt.html</t>
+  </si>
+  <si>
+    <t>Błękitna Fala</t>
+  </si>
+  <si>
+    <t>biuro@blekitna.com</t>
+  </si>
+  <si>
+    <t>Best Tailor</t>
+  </si>
+  <si>
+    <t>biuro@best-tailor.pl</t>
+  </si>
+  <si>
+    <t>https://www.best-tailor.pl/en/contact/</t>
+  </si>
+  <si>
+    <t>seisan@seisan.pl</t>
+  </si>
+  <si>
+    <t>Seisan</t>
+  </si>
+  <si>
+    <t>https://seisan.pl/pl/kontakt/</t>
+  </si>
+  <si>
+    <t>https://firmyspozywcze.pl/</t>
+  </si>
+  <si>
+    <t>Produkcja żywności</t>
+  </si>
+  <si>
+    <t>https://pupilfoods.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>Pupil Foods</t>
+  </si>
+  <si>
+    <t>info@pupilfoods.pl</t>
+  </si>
+  <si>
+    <t>Sante</t>
+  </si>
+  <si>
+    <t>https://sante.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>b2b@sante.pl</t>
+  </si>
+  <si>
+    <t>FeedPro</t>
+  </si>
+  <si>
+    <t>https://feedpro.pl/</t>
+  </si>
+  <si>
+    <t>info@feedpro.pl</t>
+  </si>
+  <si>
+    <t>Poland Tastes Goodhttps://www.polandtastesgood.pl/pl/kontakt/eksporter@kowr.gov.pl</t>
+  </si>
+  <si>
+    <t>eksporter@kowr.gov.pl</t>
+  </si>
+  <si>
+    <t>https://www.polandtastesgood.pl/pl/kontakt/</t>
+  </si>
+  <si>
+    <t>https://polskiekonto.pl/polskie-firmy-spozywcze/</t>
+  </si>
+  <si>
+    <t>https://www.primavika.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>Primavika</t>
+  </si>
+  <si>
+    <t>kontakt@primavika.pl</t>
+  </si>
+  <si>
+    <t>Janex</t>
+  </si>
+  <si>
+    <t>info@janexfoods.com</t>
+  </si>
+  <si>
+    <t>https://janexfoods.com/en/homepage/</t>
+  </si>
+  <si>
+    <t>Agilery</t>
+  </si>
+  <si>
+    <t>https://agileryfood.com/pl/#hubspotForm</t>
+  </si>
+  <si>
+    <t>hello@agilery.ch</t>
+  </si>
+  <si>
+    <t>https://klasyfikacje.gofin.pl/pkd/5,2,1443,produkcja-artykulow-spozywczych.html</t>
+  </si>
+  <si>
+    <t>https://www.emis.com/</t>
+  </si>
+  <si>
+    <t>Lyo</t>
+  </si>
+  <si>
+    <t>info@lyofood.com</t>
+  </si>
+  <si>
+    <t>https://lyofood.pl/pages/contact</t>
+  </si>
+  <si>
+    <t>Ślimak Food Servicehttps://www.slimak.com.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>biuro@slimak.com.pl</t>
+  </si>
+  <si>
+    <t>https://www.lunching.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>Lunching</t>
+  </si>
+  <si>
+    <t>partnerzy@lunching.pl</t>
+  </si>
+  <si>
+    <t>Kupiec</t>
+  </si>
+  <si>
+    <t>sekretariat@kupiec.pl</t>
+  </si>
+  <si>
+    <t>https://kupiec.pl/pl/content/10-kontakt</t>
+  </si>
+  <si>
+    <t>https://www.smartlunch.pl/kontakt</t>
+  </si>
+  <si>
+    <t>piotr.sienkiewicz@smartlunch.pl</t>
+  </si>
+  <si>
+    <t>Smart Lunch</t>
+  </si>
+  <si>
+    <t>https://factories.pl/</t>
+  </si>
+  <si>
+    <t>Rachunkowość</t>
+  </si>
+  <si>
+    <t>https://www.nex.katowice.pl/kontakt</t>
+  </si>
+  <si>
+    <t>biuro@nex.katowice.pl</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>Open Profit</t>
+  </si>
+  <si>
+    <t>biuro_op@openprofit.pl</t>
+  </si>
+  <si>
+    <t>https://openprofit.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>kderela@glc.pl</t>
+  </si>
+  <si>
+    <t>Klaudia</t>
+  </si>
+  <si>
+    <t>GLC</t>
+  </si>
+  <si>
+    <t>https://glc.pl/ksiegowosc/</t>
+  </si>
+  <si>
+    <t>Getsix</t>
+  </si>
+  <si>
+    <t>https://getsix.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>katowice@getsix.pl</t>
+  </si>
+  <si>
+    <t>Monika</t>
+  </si>
+  <si>
+    <t>Fresz</t>
+  </si>
+  <si>
+    <t>https://e-fresz.com.pl/kontakt</t>
+  </si>
+  <si>
+    <t>biuro@e-fresz.com.pl</t>
+  </si>
+  <si>
+    <t>ASK-Finance</t>
+  </si>
+  <si>
+    <t>biuro@ask-finance.pl</t>
+  </si>
+  <si>
+    <t>https://ask-finance.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>Centrum Księgowe</t>
+  </si>
+  <si>
+    <t>kontakt@centrumksiegowe.pl</t>
+  </si>
+  <si>
+    <t>https://centrumksiegowe.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>Volenti</t>
+  </si>
+  <si>
+    <t>sekretariat@volenti.pl</t>
+  </si>
+  <si>
+    <t>https://volenti.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>Warido</t>
+  </si>
+  <si>
+    <t>sekretariat@warido.com</t>
+  </si>
+  <si>
+    <t>https://warido.com/kontakt/</t>
+  </si>
+  <si>
+    <t>https://www.oferteo.pl/biuro-rachunkowe</t>
+  </si>
+  <si>
+    <t>Piotr</t>
+  </si>
+  <si>
+    <t>SII</t>
+  </si>
+  <si>
+    <t>https://sii.pl/contact-us/</t>
+  </si>
+  <si>
+    <t>contact@sii.pl</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>https://zrobotyzowany.pl/</t>
+  </si>
+  <si>
+    <t>Aiut</t>
+  </si>
+  <si>
+    <t>crm_team@aiut.com</t>
+  </si>
+  <si>
+    <t>Astor</t>
+  </si>
+  <si>
+    <t>wojciech.trojniar@astor.com.pl</t>
+  </si>
+  <si>
+    <t>Wojciech</t>
+  </si>
+  <si>
+    <t>info@baumalog.pl</t>
+  </si>
+  <si>
+    <t>Baumalog</t>
+  </si>
+  <si>
+    <t>info.pl@ifm.com</t>
+  </si>
+  <si>
+    <t>Ifm</t>
+  </si>
+  <si>
+    <t>Lenze</t>
+  </si>
+  <si>
+    <t>biuro.pl@lenze.com</t>
+  </si>
+  <si>
+    <t>sales@scramjet.org</t>
+  </si>
+  <si>
+    <t>Scramjet</t>
+  </si>
+  <si>
+    <t>Big Data &amp; Analytics</t>
+  </si>
+  <si>
+    <t>Inetum</t>
+  </si>
+  <si>
+    <t>poland@inetum.com</t>
+  </si>
+  <si>
+    <t>https://inetum.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>Britenet</t>
+  </si>
+  <si>
+    <t>office@britenet.eu</t>
+  </si>
+  <si>
+    <t>https://britenet.eu/contact/</t>
+  </si>
+  <si>
+    <t>Avenga</t>
+  </si>
+  <si>
+    <t>hello@avenga.com</t>
+  </si>
+  <si>
+    <t>https://www.avenga.com/contact-avenga/?region=pl</t>
+  </si>
+  <si>
+    <t>https://www.future-processing.com/contact/</t>
+  </si>
+  <si>
+    <t>Future Processing</t>
+  </si>
+  <si>
+    <t>sales@future-processing.com</t>
+  </si>
+  <si>
+    <t>Dawid</t>
+  </si>
+  <si>
+    <t>Getindata</t>
+  </si>
+  <si>
+    <t>hello@getindata.com</t>
+  </si>
+  <si>
+    <t>https://getindata.com/</t>
+  </si>
+  <si>
+    <t>Edvantis</t>
+  </si>
+  <si>
+    <t>engagement@edvantis.com</t>
+  </si>
+  <si>
+    <t>https://www.edvantis.com/contact-us/</t>
+  </si>
+  <si>
+    <t>Tigers</t>
+  </si>
+  <si>
+    <t>karol.jaworski@tigers.pl</t>
+  </si>
+  <si>
+    <t>Karol</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -46,13 +568,70 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF1C1C1C"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3DAC9E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -64,13 +643,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,12 +996,883 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85A562B-1E12-F248-9F6A-9CC2DF16FAA0}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="185" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" t="s">
+        <v>116</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" t="s">
+        <v>124</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" t="s">
+        <v>127</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>138</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>145</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" t="s">
+        <v>147</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>150</v>
+      </c>
+      <c r="C47" t="s">
+        <v>152</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F47" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" t="s">
+        <v>155</v>
+      </c>
+      <c r="D48" t="s">
+        <v>154</v>
+      </c>
+      <c r="F48" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>156</v>
+      </c>
+      <c r="C49" t="s">
+        <v>158</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" t="s">
+        <v>159</v>
+      </c>
+      <c r="D50" t="s">
+        <v>161</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F50" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>163</v>
+      </c>
+      <c r="C51" t="s">
+        <v>165</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F51" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" t="s">
+        <v>168</v>
+      </c>
+      <c r="D52" t="s">
+        <v>167</v>
+      </c>
+      <c r="F52" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>169</v>
+      </c>
+      <c r="D53" t="s">
+        <v>170</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F53" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="mailto:biuro@reflect.pl" xr:uid="{1473D7D8-6027-0147-9114-0C843A88EEA8}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{2B161E36-E325-754B-A9A6-3BDA6067325F}"/>
+    <hyperlink ref="D4" r:id="rId3" tooltip="Kontakt z nami" display="mailto:biuro@4lans.pl" xr:uid="{E28CB2BD-F70D-EB4A-A456-36214491536A}"/>
+    <hyperlink ref="D6" r:id="rId4" display="mailto:hello@rascalindustry.eu" xr:uid="{541189CD-8398-F849-9AD4-70018A8B06E4}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{1C83302B-0B3F-CF4F-BFD2-CD81A72A2C74}"/>
+    <hyperlink ref="D8" r:id="rId6" display="mailto:info@artdress.com.pl" xr:uid="{5672FC98-487B-D344-AA8E-33B50729AA55}"/>
+    <hyperlink ref="D9" r:id="rId7" display="mailto:elastic@elastic.com.pl" xr:uid="{E05DD2E2-E9E2-354F-8C47-6F220A23B118}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{2D205B73-F70E-7147-B23B-DA8C210AA345}"/>
+    <hyperlink ref="C11" r:id="rId9" xr:uid="{DF7493C6-11C1-B644-936D-F5FD142923D9}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{066C1328-2E1C-684D-99C7-2A1E3B7732AE}"/>
+    <hyperlink ref="D12" r:id="rId11" display="mailto:fabris@fabris.pl" xr:uid="{061A8AA6-1DC3-0344-BC68-5ACCA3C69A87}"/>
+    <hyperlink ref="D14" r:id="rId12" display="mailto:hello@bluzup.com" xr:uid="{ED4D5468-E1B8-AF40-A4A9-80AFB712BCDA}"/>
+    <hyperlink ref="C7" r:id="rId13" xr:uid="{23AA0291-2469-2140-9576-936FD755C5EF}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{5A472D6C-3442-8643-A315-0990F3FD2558}"/>
+    <hyperlink ref="C15" r:id="rId15" xr:uid="{7B9A7FF6-DE70-444E-930C-8C188496E5CD}"/>
+    <hyperlink ref="D17" r:id="rId16" display="mailto:biuro@best-tailor.pl" xr:uid="{1AB56BC4-E08C-0A45-8818-0A81BB01922C}"/>
+    <hyperlink ref="D18" r:id="rId17" display="mailto:seisan@seisan.pl" xr:uid="{3248895A-210B-094A-853E-9C680F4F54CB}"/>
+    <hyperlink ref="D20" r:id="rId18" xr:uid="{E8659751-C643-4842-BFB7-8256EBE324E1}"/>
+    <hyperlink ref="D21" r:id="rId19" display="mailto:info@feedpro.pl" xr:uid="{574B27D0-619F-704A-9730-6C3C0E41F8EE}"/>
+    <hyperlink ref="D23" r:id="rId20" display="mailto:kontakt@primavika.pl" xr:uid="{D9B2D88E-1618-7444-9162-9F0A9F68A916}"/>
+    <hyperlink ref="D24" r:id="rId21" display="mailto:info@janexfoods.com" xr:uid="{B5216FB6-2937-654F-A50D-F153F52E1F27}"/>
+    <hyperlink ref="D25" r:id="rId22" display="mailto:hello@agilery.ch" xr:uid="{9BB13AF1-49C7-0849-AF35-91C44E0C53C3}"/>
+    <hyperlink ref="D28" r:id="rId23" display="mailto:partnerzy@lunching.pl" xr:uid="{63BEA3E9-4598-FF40-AE69-3C230047A60F}"/>
+    <hyperlink ref="D29" r:id="rId24" display="mailto:sekretariat@kupiec.pl" xr:uid="{F1551014-ED44-024F-A098-C236FA5457B8}"/>
+    <hyperlink ref="D30" r:id="rId25" display="mailto:piotr.sienkiewicz@smartlunch.pl" xr:uid="{D5E2FBBD-3EA4-894D-A3F2-BF2ABB7397F3}"/>
+    <hyperlink ref="D31" r:id="rId26" display="mailto:biuro@nex.katowice.pl" xr:uid="{0F726BCC-44F5-B843-81A7-92A76EBAC91C}"/>
+    <hyperlink ref="D32" r:id="rId27" display="mailto:biuro_op@openprofit.pl" xr:uid="{DD3BE3C7-A5D1-BC4F-9173-452423FF7ACB}"/>
+    <hyperlink ref="D33" r:id="rId28" display="mailto:kderela@glc.pl" xr:uid="{B36C74F9-E381-AC4F-B1FC-2AC35EC720E5}"/>
+    <hyperlink ref="D34" r:id="rId29" display="mailto:katowice@getsix.pl" xr:uid="{62770078-3A54-F548-9D55-69AF78C91934}"/>
+    <hyperlink ref="D36" r:id="rId30" display="mailto:biuro@ask-finance.pl" xr:uid="{01413B36-2BD2-8246-A744-9907B100A673}"/>
+    <hyperlink ref="D37" r:id="rId31" display="mailto:kontakt@centrumksiegowe.pl" xr:uid="{3F09FF0F-81D2-6C42-98C7-56247DDB41E4}"/>
+    <hyperlink ref="D41" r:id="rId32" display="mailto:crm_team@aiut.com" xr:uid="{B7BD4179-54C4-7141-BFCA-21C4B7592DA2}"/>
+    <hyperlink ref="D42" r:id="rId33" display="mailto:wojciech.trojniar@astor.com.pl" xr:uid="{BB9BF4E1-E375-824F-AED4-8C2823A67EA4}"/>
+    <hyperlink ref="D43" r:id="rId34" display="mailto:info@baumalog.pl" xr:uid="{C1EB48D6-4776-354E-B73C-2910B3879866}"/>
+    <hyperlink ref="D44" r:id="rId35" display="mailto:info.pl@ifm.com" xr:uid="{00037445-6874-BF4D-A407-7036597A1080}"/>
+    <hyperlink ref="D45" r:id="rId36" display="mailto:biuro.pl@lenze.com" xr:uid="{C4D556B5-0E5E-B94B-AF9C-7FD51A5C15CA}"/>
+    <hyperlink ref="D47" r:id="rId37" display="mailto:poland@inetum.com" xr:uid="{BCDFE1F0-1795-C74A-A2EA-362C0EC54F20}"/>
+    <hyperlink ref="D49" r:id="rId38" display="mailto:hello@avenga.com" xr:uid="{3BA4232A-22DC-8743-BE4B-84983E6D5A83}"/>
+    <hyperlink ref="D51" r:id="rId39" display="mailto:hello@getindata.com" xr:uid="{26E7C7CB-D690-914E-BD17-6C8B2FCBA833}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB52BDC-C9D8-9D47-A073-78E367AB560B}">
+  <dimension ref="B2:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>